<commit_message>
fixed adding of columns for drop down
</commit_message>
<xml_diff>
--- a/Filtered_By_Region/BARMM_NEWCON.xlsx
+++ b/Filtered_By_Region/BARMM_NEWCON.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DropdownOptions" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS48"/>
+  <dimension ref="A1:AX48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,6 +660,31 @@
           <t>Project Allocation (original)</t>
         </is>
       </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>Status as of July 4, 2025</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>Status as of July 4, 2025</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>Status as of July 4, 2025</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -697,7 +723,6 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
           <t>1-UNIT 4STY</t>
@@ -711,8 +736,6 @@
       <c r="L2" t="n">
         <v>40000000</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -721,17 +744,6 @@
       <c r="P2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="n">
         <v>0</v>
       </c>
@@ -747,7 +759,6 @@
       <c r="AF2" t="n">
         <v>0</v>
       </c>
-      <c r="AG2" t="inlineStr"/>
       <c r="AH2" t="n">
         <v>0</v>
       </c>
@@ -763,17 +774,12 @@
       <c r="AL2" t="n">
         <v>0</v>
       </c>
-      <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
         <v>0</v>
       </c>
       <c r="AO2" t="n">
         <v>0</v>
       </c>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -828,8 +834,6 @@
       <c r="L3" t="n">
         <v>40000000</v>
       </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -838,17 +842,6 @@
       <c r="P3" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
         <v>0</v>
       </c>
@@ -864,7 +857,6 @@
       <c r="AF3" t="n">
         <v>0</v>
       </c>
-      <c r="AG3" t="inlineStr"/>
       <c r="AH3" t="n">
         <v>0</v>
       </c>
@@ -880,17 +872,12 @@
       <c r="AL3" t="n">
         <v>0</v>
       </c>
-      <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
         <v>0</v>
       </c>
       <c r="AO3" t="n">
         <v>0</v>
       </c>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -911,7 +898,6 @@
       <c r="D4" t="n">
         <v>133540</v>
       </c>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>BUMBARAN</t>
@@ -941,8 +927,6 @@
       <c r="L4" t="n">
         <v>10000000</v>
       </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -951,17 +935,6 @@
       <c r="P4" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="n">
         <v>0</v>
       </c>
@@ -977,7 +950,6 @@
       <c r="AF4" t="n">
         <v>0</v>
       </c>
-      <c r="AG4" t="inlineStr"/>
       <c r="AH4" t="n">
         <v>0</v>
       </c>
@@ -993,17 +965,12 @@
       <c r="AL4" t="n">
         <v>0</v>
       </c>
-      <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="n">
         <v>0</v>
       </c>
       <c r="AO4" t="n">
         <v>0</v>
       </c>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1058,8 +1025,6 @@
       <c r="L5" t="n">
         <v>10000000</v>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1068,17 +1033,6 @@
       <c r="P5" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="n">
         <v>0</v>
       </c>
@@ -1094,7 +1048,6 @@
       <c r="AF5" t="n">
         <v>0</v>
       </c>
-      <c r="AG5" t="inlineStr"/>
       <c r="AH5" t="n">
         <v>0</v>
       </c>
@@ -1110,17 +1063,12 @@
       <c r="AL5" t="n">
         <v>0</v>
       </c>
-      <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="n">
         <v>0</v>
       </c>
       <c r="AO5" t="n">
         <v>0</v>
       </c>
-      <c r="AP5" t="inlineStr"/>
-      <c r="AQ5" t="inlineStr"/>
-      <c r="AR5" t="inlineStr"/>
-      <c r="AS5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1175,8 +1123,6 @@
       <c r="L6" t="n">
         <v>30000000</v>
       </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -1185,17 +1131,6 @@
       <c r="P6" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="n">
         <v>0</v>
       </c>
@@ -1211,7 +1146,6 @@
       <c r="AF6" t="n">
         <v>0</v>
       </c>
-      <c r="AG6" t="inlineStr"/>
       <c r="AH6" t="n">
         <v>0</v>
       </c>
@@ -1227,17 +1161,12 @@
       <c r="AL6" t="n">
         <v>0</v>
       </c>
-      <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="n">
         <v>0</v>
       </c>
       <c r="AO6" t="n">
         <v>0</v>
       </c>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="inlineStr"/>
-      <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1292,8 +1221,6 @@
       <c r="L7" t="n">
         <v>30000000</v>
       </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -1302,17 +1229,6 @@
       <c r="P7" t="n">
         <v>0</v>
       </c>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="n">
         <v>0</v>
       </c>
@@ -1328,7 +1244,6 @@
       <c r="AF7" t="n">
         <v>0</v>
       </c>
-      <c r="AG7" t="inlineStr"/>
       <c r="AH7" t="n">
         <v>0</v>
       </c>
@@ -1344,17 +1259,12 @@
       <c r="AL7" t="n">
         <v>0</v>
       </c>
-      <c r="AM7" t="inlineStr"/>
       <c r="AN7" t="n">
         <v>0</v>
       </c>
       <c r="AO7" t="n">
         <v>0</v>
       </c>
-      <c r="AP7" t="inlineStr"/>
-      <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="inlineStr"/>
-      <c r="AS7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1409,8 +1319,6 @@
       <c r="L8" t="n">
         <v>10000000</v>
       </c>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1419,17 +1327,6 @@
       <c r="P8" t="n">
         <v>0</v>
       </c>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="n">
         <v>0</v>
       </c>
@@ -1445,7 +1342,6 @@
       <c r="AF8" t="n">
         <v>0</v>
       </c>
-      <c r="AG8" t="inlineStr"/>
       <c r="AH8" t="n">
         <v>0</v>
       </c>
@@ -1461,17 +1357,12 @@
       <c r="AL8" t="n">
         <v>0</v>
       </c>
-      <c r="AM8" t="inlineStr"/>
       <c r="AN8" t="n">
         <v>0</v>
       </c>
       <c r="AO8" t="n">
         <v>0</v>
       </c>
-      <c r="AP8" t="inlineStr"/>
-      <c r="AQ8" t="inlineStr"/>
-      <c r="AR8" t="inlineStr"/>
-      <c r="AS8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1526,8 +1417,6 @@
       <c r="L9" t="n">
         <v>42000000</v>
       </c>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -1536,17 +1425,6 @@
       <c r="P9" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="n">
         <v>0</v>
       </c>
@@ -1562,7 +1440,6 @@
       <c r="AF9" t="n">
         <v>0</v>
       </c>
-      <c r="AG9" t="inlineStr"/>
       <c r="AH9" t="n">
         <v>0</v>
       </c>
@@ -1578,17 +1455,12 @@
       <c r="AL9" t="n">
         <v>0</v>
       </c>
-      <c r="AM9" t="inlineStr"/>
       <c r="AN9" t="n">
         <v>0</v>
       </c>
       <c r="AO9" t="n">
         <v>0</v>
       </c>
-      <c r="AP9" t="inlineStr"/>
-      <c r="AQ9" t="inlineStr"/>
-      <c r="AR9" t="inlineStr"/>
-      <c r="AS9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1643,8 +1515,6 @@
       <c r="L10" t="n">
         <v>10000000</v>
       </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1653,17 +1523,6 @@
       <c r="P10" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="n">
         <v>0</v>
       </c>
@@ -1679,7 +1538,6 @@
       <c r="AF10" t="n">
         <v>0</v>
       </c>
-      <c r="AG10" t="inlineStr"/>
       <c r="AH10" t="n">
         <v>0</v>
       </c>
@@ -1695,17 +1553,12 @@
       <c r="AL10" t="n">
         <v>0</v>
       </c>
-      <c r="AM10" t="inlineStr"/>
       <c r="AN10" t="n">
         <v>0</v>
       </c>
       <c r="AO10" t="n">
         <v>0</v>
       </c>
-      <c r="AP10" t="inlineStr"/>
-      <c r="AQ10" t="inlineStr"/>
-      <c r="AR10" t="inlineStr"/>
-      <c r="AS10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1760,8 +1613,6 @@
       <c r="L11" t="n">
         <v>10000000</v>
       </c>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1770,17 +1621,6 @@
       <c r="P11" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="n">
         <v>0</v>
       </c>
@@ -1796,7 +1636,6 @@
       <c r="AF11" t="n">
         <v>0</v>
       </c>
-      <c r="AG11" t="inlineStr"/>
       <c r="AH11" t="n">
         <v>0</v>
       </c>
@@ -1812,17 +1651,12 @@
       <c r="AL11" t="n">
         <v>0</v>
       </c>
-      <c r="AM11" t="inlineStr"/>
       <c r="AN11" t="n">
         <v>0</v>
       </c>
       <c r="AO11" t="n">
         <v>0</v>
       </c>
-      <c r="AP11" t="inlineStr"/>
-      <c r="AQ11" t="inlineStr"/>
-      <c r="AR11" t="inlineStr"/>
-      <c r="AS11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1877,8 +1711,6 @@
       <c r="L12" t="n">
         <v>5000000</v>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -1887,17 +1719,6 @@
       <c r="P12" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="n">
         <v>0</v>
       </c>
@@ -1913,7 +1734,6 @@
       <c r="AF12" t="n">
         <v>0</v>
       </c>
-      <c r="AG12" t="inlineStr"/>
       <c r="AH12" t="n">
         <v>0</v>
       </c>
@@ -1929,17 +1749,12 @@
       <c r="AL12" t="n">
         <v>0</v>
       </c>
-      <c r="AM12" t="inlineStr"/>
       <c r="AN12" t="n">
         <v>0</v>
       </c>
       <c r="AO12" t="n">
         <v>0</v>
       </c>
-      <c r="AP12" t="inlineStr"/>
-      <c r="AQ12" t="inlineStr"/>
-      <c r="AR12" t="inlineStr"/>
-      <c r="AS12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1957,7 +1772,6 @@
           <t>Lanao del Sur - II</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
           <t>Pagayonan National High School</t>
@@ -1992,8 +1806,6 @@
       <c r="L13" t="n">
         <v>5000000</v>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2002,17 +1814,6 @@
       <c r="P13" t="n">
         <v>0</v>
       </c>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="n">
         <v>0</v>
       </c>
@@ -2028,7 +1829,6 @@
       <c r="AF13" t="n">
         <v>0</v>
       </c>
-      <c r="AG13" t="inlineStr"/>
       <c r="AH13" t="n">
         <v>0</v>
       </c>
@@ -2044,17 +1844,12 @@
       <c r="AL13" t="n">
         <v>0</v>
       </c>
-      <c r="AM13" t="inlineStr"/>
       <c r="AN13" t="n">
         <v>0</v>
       </c>
       <c r="AO13" t="n">
         <v>0</v>
       </c>
-      <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="inlineStr"/>
-      <c r="AR13" t="inlineStr"/>
-      <c r="AS13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2109,8 +1904,6 @@
       <c r="L14" t="n">
         <v>10000000</v>
       </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2119,17 +1912,6 @@
       <c r="P14" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="n">
         <v>0</v>
       </c>
@@ -2145,7 +1927,6 @@
       <c r="AF14" t="n">
         <v>0</v>
       </c>
-      <c r="AG14" t="inlineStr"/>
       <c r="AH14" t="n">
         <v>0</v>
       </c>
@@ -2161,17 +1942,12 @@
       <c r="AL14" t="n">
         <v>0</v>
       </c>
-      <c r="AM14" t="inlineStr"/>
       <c r="AN14" t="n">
         <v>0</v>
       </c>
       <c r="AO14" t="n">
         <v>0</v>
       </c>
-      <c r="AP14" t="inlineStr"/>
-      <c r="AQ14" t="inlineStr"/>
-      <c r="AR14" t="inlineStr"/>
-      <c r="AS14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2226,8 +2002,6 @@
       <c r="L15" t="n">
         <v>5000000</v>
       </c>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2236,17 +2010,6 @@
       <c r="P15" t="n">
         <v>0</v>
       </c>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr"/>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="n">
         <v>0</v>
       </c>
@@ -2262,7 +2025,6 @@
       <c r="AF15" t="n">
         <v>0</v>
       </c>
-      <c r="AG15" t="inlineStr"/>
       <c r="AH15" t="n">
         <v>0</v>
       </c>
@@ -2278,17 +2040,12 @@
       <c r="AL15" t="n">
         <v>0</v>
       </c>
-      <c r="AM15" t="inlineStr"/>
       <c r="AN15" t="n">
         <v>0</v>
       </c>
       <c r="AO15" t="n">
         <v>0</v>
       </c>
-      <c r="AP15" t="inlineStr"/>
-      <c r="AQ15" t="inlineStr"/>
-      <c r="AR15" t="inlineStr"/>
-      <c r="AS15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2343,8 +2100,6 @@
       <c r="L16" t="n">
         <v>5000000</v>
       </c>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -2353,17 +2108,6 @@
       <c r="P16" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" t="inlineStr"/>
-      <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
-      <c r="T16" t="inlineStr"/>
-      <c r="U16" t="inlineStr"/>
-      <c r="V16" t="inlineStr"/>
-      <c r="W16" t="inlineStr"/>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="n">
         <v>0</v>
       </c>
@@ -2379,7 +2123,6 @@
       <c r="AF16" t="n">
         <v>0</v>
       </c>
-      <c r="AG16" t="inlineStr"/>
       <c r="AH16" t="n">
         <v>0</v>
       </c>
@@ -2395,17 +2138,12 @@
       <c r="AL16" t="n">
         <v>0</v>
       </c>
-      <c r="AM16" t="inlineStr"/>
       <c r="AN16" t="n">
         <v>0</v>
       </c>
       <c r="AO16" t="n">
         <v>0</v>
       </c>
-      <c r="AP16" t="inlineStr"/>
-      <c r="AQ16" t="inlineStr"/>
-      <c r="AR16" t="inlineStr"/>
-      <c r="AS16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2460,8 +2198,6 @@
       <c r="L17" t="n">
         <v>10000000</v>
       </c>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2470,17 +2206,6 @@
       <c r="P17" t="n">
         <v>0</v>
       </c>
-      <c r="Q17" t="inlineStr"/>
-      <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
-      <c r="T17" t="inlineStr"/>
-      <c r="U17" t="inlineStr"/>
-      <c r="V17" t="inlineStr"/>
-      <c r="W17" t="inlineStr"/>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="n">
         <v>0</v>
       </c>
@@ -2496,7 +2221,6 @@
       <c r="AF17" t="n">
         <v>0</v>
       </c>
-      <c r="AG17" t="inlineStr"/>
       <c r="AH17" t="n">
         <v>0</v>
       </c>
@@ -2512,17 +2236,12 @@
       <c r="AL17" t="n">
         <v>0</v>
       </c>
-      <c r="AM17" t="inlineStr"/>
       <c r="AN17" t="n">
         <v>0</v>
       </c>
       <c r="AO17" t="n">
         <v>0</v>
       </c>
-      <c r="AP17" t="inlineStr"/>
-      <c r="AQ17" t="inlineStr"/>
-      <c r="AR17" t="inlineStr"/>
-      <c r="AS17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2577,8 +2296,6 @@
       <c r="L18" t="n">
         <v>10000000</v>
       </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2587,17 +2304,6 @@
       <c r="P18" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" t="inlineStr"/>
-      <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
-      <c r="T18" t="inlineStr"/>
-      <c r="U18" t="inlineStr"/>
-      <c r="V18" t="inlineStr"/>
-      <c r="W18" t="inlineStr"/>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="n">
         <v>0</v>
       </c>
@@ -2613,7 +2319,6 @@
       <c r="AF18" t="n">
         <v>0</v>
       </c>
-      <c r="AG18" t="inlineStr"/>
       <c r="AH18" t="n">
         <v>0</v>
       </c>
@@ -2629,17 +2334,12 @@
       <c r="AL18" t="n">
         <v>0</v>
       </c>
-      <c r="AM18" t="inlineStr"/>
       <c r="AN18" t="n">
         <v>0</v>
       </c>
       <c r="AO18" t="n">
         <v>0</v>
       </c>
-      <c r="AP18" t="inlineStr"/>
-      <c r="AQ18" t="inlineStr"/>
-      <c r="AR18" t="inlineStr"/>
-      <c r="AS18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2694,8 +2394,6 @@
       <c r="L19" t="n">
         <v>10000000</v>
       </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2704,17 +2402,6 @@
       <c r="P19" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" t="inlineStr"/>
-      <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
-      <c r="T19" t="inlineStr"/>
-      <c r="U19" t="inlineStr"/>
-      <c r="V19" t="inlineStr"/>
-      <c r="W19" t="inlineStr"/>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="inlineStr"/>
-      <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="n">
         <v>0</v>
       </c>
@@ -2730,7 +2417,6 @@
       <c r="AF19" t="n">
         <v>0</v>
       </c>
-      <c r="AG19" t="inlineStr"/>
       <c r="AH19" t="n">
         <v>0</v>
       </c>
@@ -2746,17 +2432,12 @@
       <c r="AL19" t="n">
         <v>0</v>
       </c>
-      <c r="AM19" t="inlineStr"/>
       <c r="AN19" t="n">
         <v>0</v>
       </c>
       <c r="AO19" t="n">
         <v>0</v>
       </c>
-      <c r="AP19" t="inlineStr"/>
-      <c r="AQ19" t="inlineStr"/>
-      <c r="AR19" t="inlineStr"/>
-      <c r="AS19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2811,8 +2492,6 @@
       <c r="L20" t="n">
         <v>10000000</v>
       </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2821,17 +2500,6 @@
       <c r="P20" t="n">
         <v>0</v>
       </c>
-      <c r="Q20" t="inlineStr"/>
-      <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
-      <c r="T20" t="inlineStr"/>
-      <c r="U20" t="inlineStr"/>
-      <c r="V20" t="inlineStr"/>
-      <c r="W20" t="inlineStr"/>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="n">
         <v>0</v>
       </c>
@@ -2847,7 +2515,6 @@
       <c r="AF20" t="n">
         <v>0</v>
       </c>
-      <c r="AG20" t="inlineStr"/>
       <c r="AH20" t="n">
         <v>0</v>
       </c>
@@ -2863,17 +2530,12 @@
       <c r="AL20" t="n">
         <v>0</v>
       </c>
-      <c r="AM20" t="inlineStr"/>
       <c r="AN20" t="n">
         <v>0</v>
       </c>
       <c r="AO20" t="n">
         <v>0</v>
       </c>
-      <c r="AP20" t="inlineStr"/>
-      <c r="AQ20" t="inlineStr"/>
-      <c r="AR20" t="inlineStr"/>
-      <c r="AS20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2928,8 +2590,6 @@
       <c r="L21" t="n">
         <v>10000000</v>
       </c>
-      <c r="M21" t="inlineStr"/>
-      <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -2938,17 +2598,6 @@
       <c r="P21" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr"/>
-      <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="n">
         <v>0</v>
       </c>
@@ -2964,7 +2613,6 @@
       <c r="AF21" t="n">
         <v>0</v>
       </c>
-      <c r="AG21" t="inlineStr"/>
       <c r="AH21" t="n">
         <v>0</v>
       </c>
@@ -2980,17 +2628,12 @@
       <c r="AL21" t="n">
         <v>0</v>
       </c>
-      <c r="AM21" t="inlineStr"/>
       <c r="AN21" t="n">
         <v>0</v>
       </c>
       <c r="AO21" t="n">
         <v>0</v>
       </c>
-      <c r="AP21" t="inlineStr"/>
-      <c r="AQ21" t="inlineStr"/>
-      <c r="AR21" t="inlineStr"/>
-      <c r="AS21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3045,8 +2688,6 @@
       <c r="L22" t="n">
         <v>20000000</v>
       </c>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3055,17 +2696,6 @@
       <c r="P22" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
-      <c r="T22" t="inlineStr"/>
-      <c r="U22" t="inlineStr"/>
-      <c r="V22" t="inlineStr"/>
-      <c r="W22" t="inlineStr"/>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="n">
         <v>0</v>
       </c>
@@ -3081,7 +2711,6 @@
       <c r="AF22" t="n">
         <v>0</v>
       </c>
-      <c r="AG22" t="inlineStr"/>
       <c r="AH22" t="n">
         <v>0</v>
       </c>
@@ -3097,17 +2726,12 @@
       <c r="AL22" t="n">
         <v>0</v>
       </c>
-      <c r="AM22" t="inlineStr"/>
       <c r="AN22" t="n">
         <v>0</v>
       </c>
       <c r="AO22" t="n">
         <v>0</v>
       </c>
-      <c r="AP22" t="inlineStr"/>
-      <c r="AQ22" t="inlineStr"/>
-      <c r="AR22" t="inlineStr"/>
-      <c r="AS22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3125,7 +2749,6 @@
           <t>Maguindanao I</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
           <t>Tocao - Madidis National High School</t>
@@ -3160,8 +2783,6 @@
       <c r="L23" t="n">
         <v>20000000</v>
       </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3170,17 +2791,6 @@
       <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
-      <c r="T23" t="inlineStr"/>
-      <c r="U23" t="inlineStr"/>
-      <c r="V23" t="inlineStr"/>
-      <c r="W23" t="inlineStr"/>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="inlineStr"/>
-      <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="n">
         <v>0</v>
       </c>
@@ -3196,7 +2806,6 @@
       <c r="AF23" t="n">
         <v>0</v>
       </c>
-      <c r="AG23" t="inlineStr"/>
       <c r="AH23" t="n">
         <v>0</v>
       </c>
@@ -3212,17 +2821,12 @@
       <c r="AL23" t="n">
         <v>0</v>
       </c>
-      <c r="AM23" t="inlineStr"/>
       <c r="AN23" t="n">
         <v>0</v>
       </c>
       <c r="AO23" t="n">
         <v>0</v>
       </c>
-      <c r="AP23" t="inlineStr"/>
-      <c r="AQ23" t="inlineStr"/>
-      <c r="AR23" t="inlineStr"/>
-      <c r="AS23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3240,7 +2844,6 @@
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
           <t>Pura ES</t>
@@ -3275,8 +2878,6 @@
       <c r="L24" t="n">
         <v>5000000</v>
       </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3285,17 +2886,6 @@
       <c r="P24" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" t="inlineStr"/>
-      <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
-      <c r="T24" t="inlineStr"/>
-      <c r="U24" t="inlineStr"/>
-      <c r="V24" t="inlineStr"/>
-      <c r="W24" t="inlineStr"/>
-      <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="n">
         <v>0</v>
       </c>
@@ -3311,7 +2901,6 @@
       <c r="AF24" t="n">
         <v>0</v>
       </c>
-      <c r="AG24" t="inlineStr"/>
       <c r="AH24" t="n">
         <v>0</v>
       </c>
@@ -3327,17 +2916,12 @@
       <c r="AL24" t="n">
         <v>0</v>
       </c>
-      <c r="AM24" t="inlineStr"/>
       <c r="AN24" t="n">
         <v>0</v>
       </c>
       <c r="AO24" t="n">
         <v>0</v>
       </c>
-      <c r="AP24" t="inlineStr"/>
-      <c r="AQ24" t="inlineStr"/>
-      <c r="AR24" t="inlineStr"/>
-      <c r="AS24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3392,8 +2976,6 @@
       <c r="L25" t="n">
         <v>5000000</v>
       </c>
-      <c r="M25" t="inlineStr"/>
-      <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3402,17 +2984,6 @@
       <c r="P25" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="inlineStr"/>
-      <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
-      <c r="T25" t="inlineStr"/>
-      <c r="U25" t="inlineStr"/>
-      <c r="V25" t="inlineStr"/>
-      <c r="W25" t="inlineStr"/>
-      <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="inlineStr"/>
-      <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="n">
         <v>0</v>
       </c>
@@ -3428,7 +2999,6 @@
       <c r="AF25" t="n">
         <v>0</v>
       </c>
-      <c r="AG25" t="inlineStr"/>
       <c r="AH25" t="n">
         <v>0</v>
       </c>
@@ -3444,17 +3014,12 @@
       <c r="AL25" t="n">
         <v>0</v>
       </c>
-      <c r="AM25" t="inlineStr"/>
       <c r="AN25" t="n">
         <v>0</v>
       </c>
       <c r="AO25" t="n">
         <v>0</v>
       </c>
-      <c r="AP25" t="inlineStr"/>
-      <c r="AQ25" t="inlineStr"/>
-      <c r="AR25" t="inlineStr"/>
-      <c r="AS25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3509,8 +3074,6 @@
       <c r="L26" t="n">
         <v>5000000</v>
       </c>
-      <c r="M26" t="inlineStr"/>
-      <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3519,17 +3082,6 @@
       <c r="P26" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" t="inlineStr"/>
-      <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
-      <c r="T26" t="inlineStr"/>
-      <c r="U26" t="inlineStr"/>
-      <c r="V26" t="inlineStr"/>
-      <c r="W26" t="inlineStr"/>
-      <c r="X26" t="inlineStr"/>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="n">
         <v>0</v>
       </c>
@@ -3545,7 +3097,6 @@
       <c r="AF26" t="n">
         <v>0</v>
       </c>
-      <c r="AG26" t="inlineStr"/>
       <c r="AH26" t="n">
         <v>0</v>
       </c>
@@ -3561,17 +3112,12 @@
       <c r="AL26" t="n">
         <v>0</v>
       </c>
-      <c r="AM26" t="inlineStr"/>
       <c r="AN26" t="n">
         <v>0</v>
       </c>
       <c r="AO26" t="n">
         <v>0</v>
       </c>
-      <c r="AP26" t="inlineStr"/>
-      <c r="AQ26" t="inlineStr"/>
-      <c r="AR26" t="inlineStr"/>
-      <c r="AS26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3589,7 +3135,6 @@
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
           <t>Bayanga Norte ES</t>
@@ -3624,8 +3169,6 @@
       <c r="L27" t="n">
         <v>5000000</v>
       </c>
-      <c r="M27" t="inlineStr"/>
-      <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3634,17 +3177,6 @@
       <c r="P27" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" t="inlineStr"/>
-      <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
-      <c r="T27" t="inlineStr"/>
-      <c r="U27" t="inlineStr"/>
-      <c r="V27" t="inlineStr"/>
-      <c r="W27" t="inlineStr"/>
-      <c r="X27" t="inlineStr"/>
-      <c r="Y27" t="inlineStr"/>
-      <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="n">
         <v>0</v>
       </c>
@@ -3660,7 +3192,6 @@
       <c r="AF27" t="n">
         <v>0</v>
       </c>
-      <c r="AG27" t="inlineStr"/>
       <c r="AH27" t="n">
         <v>0</v>
       </c>
@@ -3676,17 +3207,12 @@
       <c r="AL27" t="n">
         <v>0</v>
       </c>
-      <c r="AM27" t="inlineStr"/>
       <c r="AN27" t="n">
         <v>0</v>
       </c>
       <c r="AO27" t="n">
         <v>0</v>
       </c>
-      <c r="AP27" t="inlineStr"/>
-      <c r="AQ27" t="inlineStr"/>
-      <c r="AR27" t="inlineStr"/>
-      <c r="AS27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3741,8 +3267,6 @@
       <c r="L28" t="n">
         <v>5000000</v>
       </c>
-      <c r="M28" t="inlineStr"/>
-      <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3751,17 +3275,6 @@
       <c r="P28" t="n">
         <v>0</v>
       </c>
-      <c r="Q28" t="inlineStr"/>
-      <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
-      <c r="T28" t="inlineStr"/>
-      <c r="U28" t="inlineStr"/>
-      <c r="V28" t="inlineStr"/>
-      <c r="W28" t="inlineStr"/>
-      <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
-      <c r="Z28" t="inlineStr"/>
-      <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="n">
         <v>0</v>
       </c>
@@ -3777,7 +3290,6 @@
       <c r="AF28" t="n">
         <v>0</v>
       </c>
-      <c r="AG28" t="inlineStr"/>
       <c r="AH28" t="n">
         <v>0</v>
       </c>
@@ -3793,17 +3305,12 @@
       <c r="AL28" t="n">
         <v>0</v>
       </c>
-      <c r="AM28" t="inlineStr"/>
       <c r="AN28" t="n">
         <v>0</v>
       </c>
       <c r="AO28" t="n">
         <v>0</v>
       </c>
-      <c r="AP28" t="inlineStr"/>
-      <c r="AQ28" t="inlineStr"/>
-      <c r="AR28" t="inlineStr"/>
-      <c r="AS28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3858,8 +3365,6 @@
       <c r="L29" t="n">
         <v>5000000</v>
       </c>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3868,17 +3373,6 @@
       <c r="P29" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" t="inlineStr"/>
-      <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr"/>
-      <c r="U29" t="inlineStr"/>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr"/>
-      <c r="X29" t="inlineStr"/>
-      <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
-      <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="n">
         <v>0</v>
       </c>
@@ -3894,7 +3388,6 @@
       <c r="AF29" t="n">
         <v>0</v>
       </c>
-      <c r="AG29" t="inlineStr"/>
       <c r="AH29" t="n">
         <v>0</v>
       </c>
@@ -3910,17 +3403,12 @@
       <c r="AL29" t="n">
         <v>0</v>
       </c>
-      <c r="AM29" t="inlineStr"/>
       <c r="AN29" t="n">
         <v>0</v>
       </c>
       <c r="AO29" t="n">
         <v>0</v>
       </c>
-      <c r="AP29" t="inlineStr"/>
-      <c r="AQ29" t="inlineStr"/>
-      <c r="AR29" t="inlineStr"/>
-      <c r="AS29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3938,7 +3426,6 @@
           <t>Maguindanao II</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
           <t>Inawan ES</t>
@@ -3973,8 +3460,6 @@
       <c r="L30" t="n">
         <v>5000000</v>
       </c>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -3983,17 +3468,6 @@
       <c r="P30" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" t="inlineStr"/>
-      <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
-      <c r="T30" t="inlineStr"/>
-      <c r="U30" t="inlineStr"/>
-      <c r="V30" t="inlineStr"/>
-      <c r="W30" t="inlineStr"/>
-      <c r="X30" t="inlineStr"/>
-      <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
-      <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="n">
         <v>0</v>
       </c>
@@ -4009,7 +3483,6 @@
       <c r="AF30" t="n">
         <v>0</v>
       </c>
-      <c r="AG30" t="inlineStr"/>
       <c r="AH30" t="n">
         <v>0</v>
       </c>
@@ -4025,17 +3498,12 @@
       <c r="AL30" t="n">
         <v>0</v>
       </c>
-      <c r="AM30" t="inlineStr"/>
       <c r="AN30" t="n">
         <v>0</v>
       </c>
       <c r="AO30" t="n">
         <v>0</v>
       </c>
-      <c r="AP30" t="inlineStr"/>
-      <c r="AQ30" t="inlineStr"/>
-      <c r="AR30" t="inlineStr"/>
-      <c r="AS30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4090,8 +3558,6 @@
       <c r="L31" t="n">
         <v>5000000</v>
       </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4100,17 +3566,6 @@
       <c r="P31" t="n">
         <v>0</v>
       </c>
-      <c r="Q31" t="inlineStr"/>
-      <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
-      <c r="T31" t="inlineStr"/>
-      <c r="U31" t="inlineStr"/>
-      <c r="V31" t="inlineStr"/>
-      <c r="W31" t="inlineStr"/>
-      <c r="X31" t="inlineStr"/>
-      <c r="Y31" t="inlineStr"/>
-      <c r="Z31" t="inlineStr"/>
-      <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="n">
         <v>0</v>
       </c>
@@ -4126,7 +3581,6 @@
       <c r="AF31" t="n">
         <v>0</v>
       </c>
-      <c r="AG31" t="inlineStr"/>
       <c r="AH31" t="n">
         <v>0</v>
       </c>
@@ -4142,17 +3596,12 @@
       <c r="AL31" t="n">
         <v>0</v>
       </c>
-      <c r="AM31" t="inlineStr"/>
       <c r="AN31" t="n">
         <v>0</v>
       </c>
       <c r="AO31" t="n">
         <v>0</v>
       </c>
-      <c r="AP31" t="inlineStr"/>
-      <c r="AQ31" t="inlineStr"/>
-      <c r="AR31" t="inlineStr"/>
-      <c r="AS31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4207,8 +3656,6 @@
       <c r="L32" t="n">
         <v>42000000</v>
       </c>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -4217,17 +3664,6 @@
       <c r="P32" t="n">
         <v>0</v>
       </c>
-      <c r="Q32" t="inlineStr"/>
-      <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
-      <c r="T32" t="inlineStr"/>
-      <c r="U32" t="inlineStr"/>
-      <c r="V32" t="inlineStr"/>
-      <c r="W32" t="inlineStr"/>
-      <c r="X32" t="inlineStr"/>
-      <c r="Y32" t="inlineStr"/>
-      <c r="Z32" t="inlineStr"/>
-      <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="n">
         <v>0</v>
       </c>
@@ -4243,7 +3679,6 @@
       <c r="AF32" t="n">
         <v>0</v>
       </c>
-      <c r="AG32" t="inlineStr"/>
       <c r="AH32" t="n">
         <v>0</v>
       </c>
@@ -4259,17 +3694,12 @@
       <c r="AL32" t="n">
         <v>0</v>
       </c>
-      <c r="AM32" t="inlineStr"/>
       <c r="AN32" t="n">
         <v>0</v>
       </c>
       <c r="AO32" t="n">
         <v>0</v>
       </c>
-      <c r="AP32" t="inlineStr"/>
-      <c r="AQ32" t="inlineStr"/>
-      <c r="AR32" t="inlineStr"/>
-      <c r="AS32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4324,8 +3754,6 @@
       <c r="L33" t="n">
         <v>10000000</v>
       </c>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4334,17 +3762,6 @@
       <c r="P33" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" t="inlineStr"/>
-      <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr"/>
-      <c r="U33" t="inlineStr"/>
-      <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
-      <c r="X33" t="inlineStr"/>
-      <c r="Y33" t="inlineStr"/>
-      <c r="Z33" t="inlineStr"/>
-      <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="n">
         <v>0</v>
       </c>
@@ -4360,7 +3777,6 @@
       <c r="AF33" t="n">
         <v>0</v>
       </c>
-      <c r="AG33" t="inlineStr"/>
       <c r="AH33" t="n">
         <v>0</v>
       </c>
@@ -4376,17 +3792,12 @@
       <c r="AL33" t="n">
         <v>0</v>
       </c>
-      <c r="AM33" t="inlineStr"/>
       <c r="AN33" t="n">
         <v>0</v>
       </c>
       <c r="AO33" t="n">
         <v>0</v>
       </c>
-      <c r="AP33" t="inlineStr"/>
-      <c r="AQ33" t="inlineStr"/>
-      <c r="AR33" t="inlineStr"/>
-      <c r="AS33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4404,7 +3815,6 @@
           <t>Sulu</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
           <t>Sultan Jamalul Kiram Central High School</t>
@@ -4439,8 +3849,6 @@
       <c r="L34" t="n">
         <v>40000000</v>
       </c>
-      <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4449,17 +3857,6 @@
       <c r="P34" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="inlineStr"/>
-      <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
-      <c r="T34" t="inlineStr"/>
-      <c r="U34" t="inlineStr"/>
-      <c r="V34" t="inlineStr"/>
-      <c r="W34" t="inlineStr"/>
-      <c r="X34" t="inlineStr"/>
-      <c r="Y34" t="inlineStr"/>
-      <c r="Z34" t="inlineStr"/>
-      <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="n">
         <v>0</v>
       </c>
@@ -4475,7 +3872,6 @@
       <c r="AF34" t="n">
         <v>0</v>
       </c>
-      <c r="AG34" t="inlineStr"/>
       <c r="AH34" t="n">
         <v>0</v>
       </c>
@@ -4491,17 +3887,12 @@
       <c r="AL34" t="n">
         <v>0</v>
       </c>
-      <c r="AM34" t="inlineStr"/>
       <c r="AN34" t="n">
         <v>0</v>
       </c>
       <c r="AO34" t="n">
         <v>0</v>
       </c>
-      <c r="AP34" t="inlineStr"/>
-      <c r="AQ34" t="inlineStr"/>
-      <c r="AR34" t="inlineStr"/>
-      <c r="AS34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4519,7 +3910,6 @@
           <t>Sulu</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
           <t>Patikul NHS - Extension</t>
@@ -4554,8 +3944,6 @@
       <c r="L35" t="n">
         <v>10000000</v>
       </c>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4564,17 +3952,6 @@
       <c r="P35" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
-      <c r="V35" t="inlineStr"/>
-      <c r="W35" t="inlineStr"/>
-      <c r="X35" t="inlineStr"/>
-      <c r="Y35" t="inlineStr"/>
-      <c r="Z35" t="inlineStr"/>
-      <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="n">
         <v>0</v>
       </c>
@@ -4590,7 +3967,6 @@
       <c r="AF35" t="n">
         <v>0</v>
       </c>
-      <c r="AG35" t="inlineStr"/>
       <c r="AH35" t="n">
         <v>0</v>
       </c>
@@ -4606,17 +3982,12 @@
       <c r="AL35" t="n">
         <v>0</v>
       </c>
-      <c r="AM35" t="inlineStr"/>
       <c r="AN35" t="n">
         <v>0</v>
       </c>
       <c r="AO35" t="n">
         <v>0</v>
       </c>
-      <c r="AP35" t="inlineStr"/>
-      <c r="AQ35" t="inlineStr"/>
-      <c r="AR35" t="inlineStr"/>
-      <c r="AS35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4671,8 +4042,6 @@
       <c r="L36" t="n">
         <v>40000000</v>
       </c>
-      <c r="M36" t="inlineStr"/>
-      <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -4681,17 +4050,6 @@
       <c r="P36" t="n">
         <v>0</v>
       </c>
-      <c r="Q36" t="inlineStr"/>
-      <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
-      <c r="T36" t="inlineStr"/>
-      <c r="U36" t="inlineStr"/>
-      <c r="V36" t="inlineStr"/>
-      <c r="W36" t="inlineStr"/>
-      <c r="X36" t="inlineStr"/>
-      <c r="Y36" t="inlineStr"/>
-      <c r="Z36" t="inlineStr"/>
-      <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="n">
         <v>0</v>
       </c>
@@ -4707,7 +4065,6 @@
       <c r="AF36" t="n">
         <v>0</v>
       </c>
-      <c r="AG36" t="inlineStr"/>
       <c r="AH36" t="n">
         <v>0</v>
       </c>
@@ -4723,17 +4080,12 @@
       <c r="AL36" t="n">
         <v>0</v>
       </c>
-      <c r="AM36" t="inlineStr"/>
       <c r="AN36" t="n">
         <v>0</v>
       </c>
       <c r="AO36" t="n">
         <v>0</v>
       </c>
-      <c r="AP36" t="inlineStr"/>
-      <c r="AQ36" t="inlineStr"/>
-      <c r="AR36" t="inlineStr"/>
-      <c r="AS36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4788,8 +4140,6 @@
       <c r="L37" t="n">
         <v>7329687.55</v>
       </c>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -4798,17 +4148,6 @@
       <c r="P37" t="n">
         <v>0</v>
       </c>
-      <c r="Q37" t="inlineStr"/>
-      <c r="R37" t="inlineStr"/>
-      <c r="S37" t="inlineStr"/>
-      <c r="T37" t="inlineStr"/>
-      <c r="U37" t="inlineStr"/>
-      <c r="V37" t="inlineStr"/>
-      <c r="W37" t="inlineStr"/>
-      <c r="X37" t="inlineStr"/>
-      <c r="Y37" t="inlineStr"/>
-      <c r="Z37" t="inlineStr"/>
-      <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="n">
         <v>0</v>
       </c>
@@ -4824,7 +4163,6 @@
       <c r="AF37" t="n">
         <v>0</v>
       </c>
-      <c r="AG37" t="inlineStr"/>
       <c r="AH37" t="n">
         <v>0</v>
       </c>
@@ -4840,17 +4178,12 @@
       <c r="AL37" t="n">
         <v>0</v>
       </c>
-      <c r="AM37" t="inlineStr"/>
       <c r="AN37" t="n">
         <v>0</v>
       </c>
       <c r="AO37" t="n">
         <v>0</v>
       </c>
-      <c r="AP37" t="inlineStr"/>
-      <c r="AQ37" t="inlineStr"/>
-      <c r="AR37" t="inlineStr"/>
-      <c r="AS37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4905,8 +4238,6 @@
       <c r="L38" t="n">
         <v>7329687.55</v>
       </c>
-      <c r="M38" t="inlineStr"/>
-      <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -4915,17 +4246,6 @@
       <c r="P38" t="n">
         <v>0</v>
       </c>
-      <c r="Q38" t="inlineStr"/>
-      <c r="R38" t="inlineStr"/>
-      <c r="S38" t="inlineStr"/>
-      <c r="T38" t="inlineStr"/>
-      <c r="U38" t="inlineStr"/>
-      <c r="V38" t="inlineStr"/>
-      <c r="W38" t="inlineStr"/>
-      <c r="X38" t="inlineStr"/>
-      <c r="Y38" t="inlineStr"/>
-      <c r="Z38" t="inlineStr"/>
-      <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="n">
         <v>0</v>
       </c>
@@ -4941,7 +4261,6 @@
       <c r="AF38" t="n">
         <v>0</v>
       </c>
-      <c r="AG38" t="inlineStr"/>
       <c r="AH38" t="n">
         <v>0</v>
       </c>
@@ -4957,17 +4276,12 @@
       <c r="AL38" t="n">
         <v>0</v>
       </c>
-      <c r="AM38" t="inlineStr"/>
       <c r="AN38" t="n">
         <v>0</v>
       </c>
       <c r="AO38" t="n">
         <v>0</v>
       </c>
-      <c r="AP38" t="inlineStr"/>
-      <c r="AQ38" t="inlineStr"/>
-      <c r="AR38" t="inlineStr"/>
-      <c r="AS38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5022,8 +4336,6 @@
       <c r="L39" t="n">
         <v>5670312.45</v>
       </c>
-      <c r="M39" t="inlineStr"/>
-      <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -5032,17 +4344,6 @@
       <c r="P39" t="n">
         <v>0</v>
       </c>
-      <c r="Q39" t="inlineStr"/>
-      <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
-      <c r="T39" t="inlineStr"/>
-      <c r="U39" t="inlineStr"/>
-      <c r="V39" t="inlineStr"/>
-      <c r="W39" t="inlineStr"/>
-      <c r="X39" t="inlineStr"/>
-      <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
-      <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="n">
         <v>0</v>
       </c>
@@ -5058,7 +4359,6 @@
       <c r="AF39" t="n">
         <v>0</v>
       </c>
-      <c r="AG39" t="inlineStr"/>
       <c r="AH39" t="n">
         <v>0</v>
       </c>
@@ -5074,17 +4374,12 @@
       <c r="AL39" t="n">
         <v>0</v>
       </c>
-      <c r="AM39" t="inlineStr"/>
       <c r="AN39" t="n">
         <v>0</v>
       </c>
       <c r="AO39" t="n">
         <v>0</v>
       </c>
-      <c r="AP39" t="inlineStr"/>
-      <c r="AQ39" t="inlineStr"/>
-      <c r="AR39" t="inlineStr"/>
-      <c r="AS39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5139,8 +4434,6 @@
       <c r="L40" t="n">
         <v>5670312.45</v>
       </c>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr">
         <is>
           <t>On Going</t>
@@ -5149,17 +4442,6 @@
       <c r="P40" t="n">
         <v>0</v>
       </c>
-      <c r="Q40" t="inlineStr"/>
-      <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
-      <c r="T40" t="inlineStr"/>
-      <c r="U40" t="inlineStr"/>
-      <c r="V40" t="inlineStr"/>
-      <c r="W40" t="inlineStr"/>
-      <c r="X40" t="inlineStr"/>
-      <c r="Y40" t="inlineStr"/>
-      <c r="Z40" t="inlineStr"/>
-      <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="n">
         <v>0</v>
       </c>
@@ -5175,7 +4457,6 @@
       <c r="AF40" t="n">
         <v>0</v>
       </c>
-      <c r="AG40" t="inlineStr"/>
       <c r="AH40" t="n">
         <v>0</v>
       </c>
@@ -5191,17 +4472,12 @@
       <c r="AL40" t="n">
         <v>0</v>
       </c>
-      <c r="AM40" t="inlineStr"/>
       <c r="AN40" t="n">
         <v>0</v>
       </c>
       <c r="AO40" t="n">
         <v>0</v>
       </c>
-      <c r="AP40" t="inlineStr"/>
-      <c r="AQ40" t="inlineStr"/>
-      <c r="AR40" t="inlineStr"/>
-      <c r="AS40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5256,8 +4532,6 @@
       <c r="L41" t="n">
         <v>5000000</v>
       </c>
-      <c r="M41" t="inlineStr"/>
-      <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5266,17 +4540,6 @@
       <c r="P41" t="n">
         <v>0</v>
       </c>
-      <c r="Q41" t="inlineStr"/>
-      <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
-      <c r="T41" t="inlineStr"/>
-      <c r="U41" t="inlineStr"/>
-      <c r="V41" t="inlineStr"/>
-      <c r="W41" t="inlineStr"/>
-      <c r="X41" t="inlineStr"/>
-      <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr"/>
-      <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="n">
         <v>0</v>
       </c>
@@ -5292,7 +4555,6 @@
       <c r="AF41" t="n">
         <v>0</v>
       </c>
-      <c r="AG41" t="inlineStr"/>
       <c r="AH41" t="n">
         <v>0</v>
       </c>
@@ -5308,17 +4570,12 @@
       <c r="AL41" t="n">
         <v>0</v>
       </c>
-      <c r="AM41" t="inlineStr"/>
       <c r="AN41" t="n">
         <v>0</v>
       </c>
       <c r="AO41" t="n">
         <v>0</v>
       </c>
-      <c r="AP41" t="inlineStr"/>
-      <c r="AQ41" t="inlineStr"/>
-      <c r="AR41" t="inlineStr"/>
-      <c r="AS41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5373,8 +4630,6 @@
       <c r="L42" t="n">
         <v>5000000</v>
       </c>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5383,17 +4638,6 @@
       <c r="P42" t="n">
         <v>0</v>
       </c>
-      <c r="Q42" t="inlineStr"/>
-      <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
-      <c r="T42" t="inlineStr"/>
-      <c r="U42" t="inlineStr"/>
-      <c r="V42" t="inlineStr"/>
-      <c r="W42" t="inlineStr"/>
-      <c r="X42" t="inlineStr"/>
-      <c r="Y42" t="inlineStr"/>
-      <c r="Z42" t="inlineStr"/>
-      <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="n">
         <v>0</v>
       </c>
@@ -5409,7 +4653,6 @@
       <c r="AF42" t="n">
         <v>0</v>
       </c>
-      <c r="AG42" t="inlineStr"/>
       <c r="AH42" t="n">
         <v>0</v>
       </c>
@@ -5425,17 +4668,12 @@
       <c r="AL42" t="n">
         <v>0</v>
       </c>
-      <c r="AM42" t="inlineStr"/>
       <c r="AN42" t="n">
         <v>0</v>
       </c>
       <c r="AO42" t="n">
         <v>0</v>
       </c>
-      <c r="AP42" t="inlineStr"/>
-      <c r="AQ42" t="inlineStr"/>
-      <c r="AR42" t="inlineStr"/>
-      <c r="AS42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5490,8 +4728,6 @@
       <c r="L43" t="n">
         <v>5000000</v>
       </c>
-      <c r="M43" t="inlineStr"/>
-      <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5500,17 +4736,6 @@
       <c r="P43" t="n">
         <v>0</v>
       </c>
-      <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
-      <c r="T43" t="inlineStr"/>
-      <c r="U43" t="inlineStr"/>
-      <c r="V43" t="inlineStr"/>
-      <c r="W43" t="inlineStr"/>
-      <c r="X43" t="inlineStr"/>
-      <c r="Y43" t="inlineStr"/>
-      <c r="Z43" t="inlineStr"/>
-      <c r="AA43" t="inlineStr"/>
       <c r="AB43" t="n">
         <v>0</v>
       </c>
@@ -5526,7 +4751,6 @@
       <c r="AF43" t="n">
         <v>0</v>
       </c>
-      <c r="AG43" t="inlineStr"/>
       <c r="AH43" t="n">
         <v>0</v>
       </c>
@@ -5542,17 +4766,12 @@
       <c r="AL43" t="n">
         <v>0</v>
       </c>
-      <c r="AM43" t="inlineStr"/>
       <c r="AN43" t="n">
         <v>0</v>
       </c>
       <c r="AO43" t="n">
         <v>0</v>
       </c>
-      <c r="AP43" t="inlineStr"/>
-      <c r="AQ43" t="inlineStr"/>
-      <c r="AR43" t="inlineStr"/>
-      <c r="AS43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5570,7 +4789,6 @@
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
           <t>Lupah Pula CS</t>
@@ -5605,8 +4823,6 @@
       <c r="L44" t="n">
         <v>5000000</v>
       </c>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5615,17 +4831,6 @@
       <c r="P44" t="n">
         <v>0</v>
       </c>
-      <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
-      <c r="T44" t="inlineStr"/>
-      <c r="U44" t="inlineStr"/>
-      <c r="V44" t="inlineStr"/>
-      <c r="W44" t="inlineStr"/>
-      <c r="X44" t="inlineStr"/>
-      <c r="Y44" t="inlineStr"/>
-      <c r="Z44" t="inlineStr"/>
-      <c r="AA44" t="inlineStr"/>
       <c r="AB44" t="n">
         <v>0</v>
       </c>
@@ -5641,7 +4846,6 @@
       <c r="AF44" t="n">
         <v>0</v>
       </c>
-      <c r="AG44" t="inlineStr"/>
       <c r="AH44" t="n">
         <v>0</v>
       </c>
@@ -5657,17 +4861,12 @@
       <c r="AL44" t="n">
         <v>0</v>
       </c>
-      <c r="AM44" t="inlineStr"/>
       <c r="AN44" t="n">
         <v>0</v>
       </c>
       <c r="AO44" t="n">
         <v>0</v>
       </c>
-      <c r="AP44" t="inlineStr"/>
-      <c r="AQ44" t="inlineStr"/>
-      <c r="AR44" t="inlineStr"/>
-      <c r="AS44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5722,8 +4921,6 @@
       <c r="L45" t="n">
         <v>5000000</v>
       </c>
-      <c r="M45" t="inlineStr"/>
-      <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5732,17 +4929,6 @@
       <c r="P45" t="n">
         <v>0</v>
       </c>
-      <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
-      <c r="T45" t="inlineStr"/>
-      <c r="U45" t="inlineStr"/>
-      <c r="V45" t="inlineStr"/>
-      <c r="W45" t="inlineStr"/>
-      <c r="X45" t="inlineStr"/>
-      <c r="Y45" t="inlineStr"/>
-      <c r="Z45" t="inlineStr"/>
-      <c r="AA45" t="inlineStr"/>
       <c r="AB45" t="n">
         <v>0</v>
       </c>
@@ -5758,7 +4944,6 @@
       <c r="AF45" t="n">
         <v>0</v>
       </c>
-      <c r="AG45" t="inlineStr"/>
       <c r="AH45" t="n">
         <v>0</v>
       </c>
@@ -5774,17 +4959,12 @@
       <c r="AL45" t="n">
         <v>0</v>
       </c>
-      <c r="AM45" t="inlineStr"/>
       <c r="AN45" t="n">
         <v>0</v>
       </c>
       <c r="AO45" t="n">
         <v>0</v>
       </c>
-      <c r="AP45" t="inlineStr"/>
-      <c r="AQ45" t="inlineStr"/>
-      <c r="AR45" t="inlineStr"/>
-      <c r="AS45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5839,8 +5019,6 @@
       <c r="L46" t="n">
         <v>5000000</v>
       </c>
-      <c r="M46" t="inlineStr"/>
-      <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5849,17 +5027,6 @@
       <c r="P46" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
-      <c r="S46" t="inlineStr"/>
-      <c r="T46" t="inlineStr"/>
-      <c r="U46" t="inlineStr"/>
-      <c r="V46" t="inlineStr"/>
-      <c r="W46" t="inlineStr"/>
-      <c r="X46" t="inlineStr"/>
-      <c r="Y46" t="inlineStr"/>
-      <c r="Z46" t="inlineStr"/>
-      <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="n">
         <v>0</v>
       </c>
@@ -5875,7 +5042,6 @@
       <c r="AF46" t="n">
         <v>0</v>
       </c>
-      <c r="AG46" t="inlineStr"/>
       <c r="AH46" t="n">
         <v>0</v>
       </c>
@@ -5891,17 +5057,12 @@
       <c r="AL46" t="n">
         <v>0</v>
       </c>
-      <c r="AM46" t="inlineStr"/>
       <c r="AN46" t="n">
         <v>0</v>
       </c>
       <c r="AO46" t="n">
         <v>0</v>
       </c>
-      <c r="AP46" t="inlineStr"/>
-      <c r="AQ46" t="inlineStr"/>
-      <c r="AR46" t="inlineStr"/>
-      <c r="AS46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5956,8 +5117,6 @@
       <c r="L47" t="n">
         <v>5000000</v>
       </c>
-      <c r="M47" t="inlineStr"/>
-      <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -5966,17 +5125,6 @@
       <c r="P47" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
-      <c r="S47" t="inlineStr"/>
-      <c r="T47" t="inlineStr"/>
-      <c r="U47" t="inlineStr"/>
-      <c r="V47" t="inlineStr"/>
-      <c r="W47" t="inlineStr"/>
-      <c r="X47" t="inlineStr"/>
-      <c r="Y47" t="inlineStr"/>
-      <c r="Z47" t="inlineStr"/>
-      <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="n">
         <v>0</v>
       </c>
@@ -5992,7 +5140,6 @@
       <c r="AF47" t="n">
         <v>0</v>
       </c>
-      <c r="AG47" t="inlineStr"/>
       <c r="AH47" t="n">
         <v>0</v>
       </c>
@@ -6008,17 +5155,12 @@
       <c r="AL47" t="n">
         <v>0</v>
       </c>
-      <c r="AM47" t="inlineStr"/>
       <c r="AN47" t="n">
         <v>0</v>
       </c>
       <c r="AO47" t="n">
         <v>0</v>
       </c>
-      <c r="AP47" t="inlineStr"/>
-      <c r="AQ47" t="inlineStr"/>
-      <c r="AR47" t="inlineStr"/>
-      <c r="AS47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6036,7 +5178,6 @@
           <t>Tawi-Tawi</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
           <t>Tabawan Stand Alone Senior High School</t>
@@ -6071,8 +5212,6 @@
       <c r="L48" t="n">
         <v>5000000</v>
       </c>
-      <c r="M48" t="inlineStr"/>
-      <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr">
         <is>
           <t>Not Yet Started</t>
@@ -6081,17 +5220,6 @@
       <c r="P48" t="n">
         <v>0</v>
       </c>
-      <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
-      <c r="S48" t="inlineStr"/>
-      <c r="T48" t="inlineStr"/>
-      <c r="U48" t="inlineStr"/>
-      <c r="V48" t="inlineStr"/>
-      <c r="W48" t="inlineStr"/>
-      <c r="X48" t="inlineStr"/>
-      <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
-      <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="n">
         <v>0</v>
       </c>
@@ -6107,7 +5235,6 @@
       <c r="AF48" t="n">
         <v>0</v>
       </c>
-      <c r="AG48" t="inlineStr"/>
       <c r="AH48" t="n">
         <v>0</v>
       </c>
@@ -6123,17 +5250,97 @@
       <c r="AL48" t="n">
         <v>0</v>
       </c>
-      <c r="AM48" t="inlineStr"/>
       <c r="AN48" t="n">
         <v>0</v>
       </c>
       <c r="AO48" t="n">
         <v>0</v>
       </c>
-      <c r="AP48" t="inlineStr"/>
-      <c r="AQ48" t="inlineStr"/>
-      <c r="AR48" t="inlineStr"/>
-      <c r="AS48" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation sqref="AT2:AT48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=DropdownOptions!$A$1:$A$7</formula1>
+    </dataValidation>
+    <dataValidation sqref="AU2:AU48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=DropdownOptions!$A$1:$A$7</formula1>
+    </dataValidation>
+    <dataValidation sqref="AV2:AV48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=DropdownOptions!$A$1:$A$7</formula1>
+    </dataValidation>
+    <dataValidation sqref="AW2:AW48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=DropdownOptions!$A$1:$A$7</formula1>
+    </dataValidation>
+    <dataValidation sqref="AX2:AX48" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>=DropdownOptions!$A$1:$A$7</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>0% - 10%: Foundation completed: Groundwork finished; no vertical structure yet.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>11% - 25%: Structure and rough-in started: Structural framing in progress; initial MEP rough-in.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>26% - 50%: Structure erected, partial roofing: Building shape defined; roof and systems advancing.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>51% - 75%: Exterior sealed, interior work underway: Enclosed structure; painting, flooring, and testing begin.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">76% - 90%: Final finishes and inspections: Systems tested; </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>91% - 99%: Final touches and punch list: Minor adjustments; final inspections and approvals.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>100% - Construction complete: Ready for handover and occupancy.</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>